<commit_message>
labeled figures for sending
</commit_message>
<xml_diff>
--- a/data_raw/byhand_cooperator-field-size.xlsx
+++ b/data_raw/byhand_cooperator-field-size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\PFI_CanWeReduceN\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2D2942-2C44-442D-B394-790F1560F445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42AFD80-37B2-4952-8196-1AE7CF5E205E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8D98B87-03C5-485F-B357-B1A06A2B9896}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +525,9 @@
       <c r="B10">
         <v>30</v>
       </c>
+      <c r="C10">
+        <v>2010</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -570,6 +573,9 @@
       </c>
       <c r="B15">
         <v>30</v>
+      </c>
+      <c r="C15">
+        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>